<commit_message>
Change 3rd party > 3rd
</commit_message>
<xml_diff>
--- a/src/main/resources/template/3rdList.xlsx
+++ b/src/main/resources/template/3rdList.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/min/Min/ui_2.0/fosslight/src/main/resources/template/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B246D9A-CC56-2D43-BEA6-30C5C7FE4A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="24240" windowHeight="13005"/>
+    <workbookView xWindow="360" yWindow="740" windowWidth="24240" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>3rd Party Name</t>
-  </si>
-  <si>
     <t>ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -62,14 +65,18 @@
   </si>
   <si>
     <t>Division</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3rd Name</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,7 +197,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -207,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +254,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -319,7 +326,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -492,65 +499,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="18.25" customWidth="1"/>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
-    <col min="4" max="4" width="23.625" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="43.875" customWidth="1"/>
-    <col min="8" max="9" width="29.875" customWidth="1"/>
-    <col min="10" max="11" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="43.83203125" customWidth="1"/>
+    <col min="8" max="9" width="29.83203125" customWidth="1"/>
+    <col min="10" max="11" width="20.6640625" customWidth="1"/>
     <col min="12" max="12" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="18" thickBot="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -563,38 +570,47 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="B3" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>